<commit_message>
Finished updating NCRO 2022 data.
</commit_message>
<xml_diff>
--- a/data-raw/NCRO/WQDiscrete_Truckee_CY2022.xlsx
+++ b/data-raw/NCRO/WQDiscrete_Truckee_CY2022.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Water Quality Evaluation Section\Data Files\Data Request Archive\CY 2022 Discrete Data Request for RHartman\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cawater-my.sharepoint.com/personal/rosemary_hartman_water_ca_gov/Documents/DUWG/discretewq/data-raw/NCRO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{199C2E07-2DBC-4EF7-9E2C-58C5DD20CFEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{199C2E07-2DBC-4EF7-9E2C-58C5DD20CFEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6AB4D020-84AD-4689-9C4F-0A528CCD4198}"/>
   <bookViews>
-    <workbookView xWindow="28830" yWindow="-22080" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="36000" yWindow="2655" windowWidth="21600" windowHeight="12615" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1498,6 +1498,7 @@
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="3" width="46.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.35">

</xml_diff>